<commit_message>
user랑 truck 초기 모델
</commit_message>
<xml_diff>
--- a/입지 후보 선정/세척허브 입지선정/대안2_위경도.xlsx
+++ b/입지 후보 선정/세척허브 입지선정/대안2_위경도.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\오광혁\Desktop\광혁 4-1\종합설계\최종발표\세척허브 입지선정(K-means)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\오광혁\Desktop\광혁 4-1\종합설계\종설코드\입지 후보 선정\세척허브 입지선정\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A4502-796F-413B-965A-7A056428C6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B28C7E-75E9-46FC-B6E9-DCB9F50B835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{C23AAC2B-EE4B-432A-83A6-7A0730076300}"/>
+    <workbookView xWindow="680" yWindow="4140" windowWidth="19200" windowHeight="11260" activeTab="1" xr2:uid="{C23AAC2B-EE4B-432A-83A6-7A0730076300}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -422,6 +422,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1595,7 +1598,7 @@
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1609,322 +1612,322 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>37.489043100000004</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>127.02994750000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>37.509919500000002</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>127.0189443</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>37.505006450000003</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>127.00423549999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>37.491894799999997</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>126.990054</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>37.500232699999998</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>127.0173489</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>37.5031307</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>127.0112106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>37.4819478</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>126.9837912</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>37.504141500000003</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>126.99456669999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>37.503955150000003</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>127.0240414</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>37.4661185</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>127.043397</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>37.4902382</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>127.0067846</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>37.466169149999999</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>127.0328588</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>37.487273100000003</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>127.0129866</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>37.490634499999999</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>127.00959330000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>37.492290799999999</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>127.0113736</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>37.486041100000001</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>127.0135753</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>37.486372000000003</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>127.01422959999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>37.486534900000002</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>127.0125747</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>37.484926000000002</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>127.0125451</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>37.471224999999997</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>127.035042</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>37.467654000000003</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>127.030517</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>37.499763600000001</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>127.026135</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>37.481920899999999</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>127.0150625</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>37.492260700000003</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>127.01472459999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>37.501270099999999</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>127.0113085</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>37.480876299999998</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>127.0121532</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>37.482652999999999</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>127.01497310000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>37.495739399999998</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>126.9875352</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>37.469636800000004</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>127.0414121</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>37.480318099999998</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>127.0056616</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>37.504852499999998</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>127.0013227</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>37.493203200000004</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>127.00848430000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>37.5026528</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>127.016319</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>37.4990959</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>127.0000948</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>37.482929300000002</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>127.0131062</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>37.500064100000003</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>127.005228</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37.483106999999997</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>127.009331</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>37.507008999999996</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>127.022747</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>37.499369899999998</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>127.012058</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>37.485746300000002</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>127.01607</v>
       </c>
     </row>

</xml_diff>